<commit_message>
Stabile Version in Verwendung 02.06.25
</commit_message>
<xml_diff>
--- a/Monitoring/TimeMonitoring.xlsx
+++ b/Monitoring/TimeMonitoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tim/NoteDeck/Monitoring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B78C26-CBC3-A949-A75B-5822F812226F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6FD42EC-46E0-9446-AA4F-95AF4D62EBDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="181">
   <si>
     <t>Subject</t>
   </si>
@@ -602,6 +602,9 @@
   </si>
   <si>
     <t>Note</t>
+  </si>
+  <si>
+    <t>KNO</t>
   </si>
 </sst>
 </file>
@@ -839,8 +842,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F8812F56-DE6D-1C4F-8324-3BEF4B9785F9}" name="tbl_MONITORING" displayName="tbl_MONITORING" ref="C4:K5" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
-  <autoFilter ref="C4:K5" xr:uid="{F8812F56-DE6D-1C4F-8324-3BEF4B9785F9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F8812F56-DE6D-1C4F-8324-3BEF4B9785F9}" name="tbl_MONITORING" displayName="tbl_MONITORING" ref="C4:K6" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
+  <autoFilter ref="C4:K6" xr:uid="{F8812F56-DE6D-1C4F-8324-3BEF4B9785F9}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{58F4A1E6-FDF8-874F-B2B6-907AD1BEEF45}" name="Date" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{F2ACE730-A243-3942-9BEE-4173EF12B5D6}" name="Week" dataDxfId="9">
@@ -2483,10 +2486,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FF52592-4B18-4446-8693-73AD33C35A54}">
-  <dimension ref="C4:K5"/>
+  <dimension ref="C4:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2534,23 +2537,43 @@
     </row>
     <row r="5" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C5" s="3">
-        <v>45805</v>
+        <v>45806</v>
       </c>
       <c r="D5" s="2" t="str">
         <f>TEXT(WEEKNUM(tbl_MONITORING[[#This Row],[Date]], 2), "00") &amp; "-" &amp; YEAR(tbl_MONITORING[[#This Row],[Date]])</f>
         <v>22-2025</v>
       </c>
-      <c r="J5" s="4"/>
+      <c r="E5" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="J5" s="4">
+        <v>5.5555555555555552E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C6" s="3">
+        <v>45809</v>
+      </c>
+      <c r="D6" s="2" t="str">
+        <f>TEXT(WEEKNUM(tbl_MONITORING[[#This Row],[Date]], 2), "00") &amp; "-" &amp; YEAR(tbl_MONITORING[[#This Row],[Date]])</f>
+        <v>22-2025</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J6" s="4">
+        <v>5.5555555555555552E-2</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5" xr:uid="{61279C5F-07E8-7B46-9D7F-519ECF1BB30D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E6" xr:uid="{61279C5F-07E8-7B46-9D7F-519ECF1BB30D}">
       <formula1>SubjectList</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F5" xr:uid="{CAF62210-090A-B84A-96A8-13BE2B36FD85}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F6" xr:uid="{CAF62210-090A-B84A-96A8-13BE2B36FD85}">
       <formula1>LitID</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H5" xr:uid="{37CCB59F-29DE-9941-815F-B55E99067E0F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H6" xr:uid="{37CCB59F-29DE-9941-815F-B55E99067E0F}">
       <formula1>Topics</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>